<commit_message>
draft version of script to generate nsk-kdd-like features from real traffic was added
</commit_message>
<xml_diff>
--- a/Nsl_kdd_hurst_vals_for_features.xlsx
+++ b/Nsl_kdd_hurst_vals_for_features.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
-  <si>
-    <t>NSL-KDD Hurst calc</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="86">
   <si>
     <t>src_bytes</t>
   </si>
@@ -100,6 +97,183 @@
   </si>
   <si>
     <t>feature name</t>
+  </si>
+  <si>
+    <t>0.5017</t>
+  </si>
+  <si>
+    <t>0.4921</t>
+  </si>
+  <si>
+    <t>0.5160</t>
+  </si>
+  <si>
+    <t>0.5149</t>
+  </si>
+  <si>
+    <t>0.4836</t>
+  </si>
+  <si>
+    <t>0.5098</t>
+  </si>
+  <si>
+    <t>0.5457</t>
+  </si>
+  <si>
+    <t>0.5026</t>
+  </si>
+  <si>
+    <t>0.5102</t>
+  </si>
+  <si>
+    <t>0.4954</t>
+  </si>
+  <si>
+    <t>0.5303</t>
+  </si>
+  <si>
+    <t>0.5019</t>
+  </si>
+  <si>
+    <t>0.5442</t>
+  </si>
+  <si>
+    <t>0.5374</t>
+  </si>
+  <si>
+    <t>0.5511</t>
+  </si>
+  <si>
+    <t>0.5095</t>
+  </si>
+  <si>
+    <t>0.5236</t>
+  </si>
+  <si>
+    <t>wavelet analysis, matlab</t>
+  </si>
+  <si>
+    <t>0.4623</t>
+  </si>
+  <si>
+    <t>0.5246</t>
+  </si>
+  <si>
+    <t>0.4886</t>
+  </si>
+  <si>
+    <t>0.4498</t>
+  </si>
+  <si>
+    <t>0.6139</t>
+  </si>
+  <si>
+    <t>0.4865</t>
+  </si>
+  <si>
+    <t>0.5033</t>
+  </si>
+  <si>
+    <t>0.4877</t>
+  </si>
+  <si>
+    <t>0.5001</t>
+  </si>
+  <si>
+    <t>0.4931</t>
+  </si>
+  <si>
+    <t>0.5249</t>
+  </si>
+  <si>
+    <t>0.5089</t>
+  </si>
+  <si>
+    <t>0.4949</t>
+  </si>
+  <si>
+    <t>0.4932</t>
+  </si>
+  <si>
+    <t>0.4913</t>
+  </si>
+  <si>
+    <t>0.5075</t>
+  </si>
+  <si>
+    <t>0.4037</t>
+  </si>
+  <si>
+    <t>0.5211</t>
+  </si>
+  <si>
+    <t>0.4912</t>
+  </si>
+  <si>
+    <t>0.4937</t>
+  </si>
+  <si>
+    <t>0.4871</t>
+  </si>
+  <si>
+    <t>0.4855</t>
+  </si>
+  <si>
+    <t>0.4850</t>
+  </si>
+  <si>
+    <t>0.5042</t>
+  </si>
+  <si>
+    <t>0.4918</t>
+  </si>
+  <si>
+    <t>0.5097</t>
+  </si>
+  <si>
+    <t>0.4982</t>
+  </si>
+  <si>
+    <t>0.5157</t>
+  </si>
+  <si>
+    <t>0.4879</t>
+  </si>
+  <si>
+    <t>0.4888</t>
+  </si>
+  <si>
+    <t>0.4948</t>
+  </si>
+  <si>
+    <t>0.4924</t>
+  </si>
+  <si>
+    <t>0.4947</t>
+  </si>
+  <si>
+    <t>0.4503</t>
+  </si>
+  <si>
+    <t>0.5043</t>
+  </si>
+  <si>
+    <t>0.4894</t>
+  </si>
+  <si>
+    <t>0.4927</t>
+  </si>
+  <si>
+    <t>0.4901</t>
+  </si>
+  <si>
+    <t>0.4929</t>
+  </si>
+  <si>
+    <t>R/S analysis, matlab</t>
+  </si>
+  <si>
+    <t>NSL-KDD Hurst calc (R/S analysis, python)</t>
   </si>
 </sst>
 </file>
@@ -152,7 +326,41 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -181,8 +389,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A2:D16" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="A2:D16" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A2:D16"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="feature name"/>
+    <tableColumn id="2" name="normal H"/>
+    <tableColumn id="3" name="attack H"/>
+    <tableColumn id="4" name="full H"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица22" displayName="Таблица22" ref="A20:D34" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A20:D34"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="feature name"/>
+    <tableColumn id="2" name="normal H"/>
+    <tableColumn id="3" name="attack H"/>
+    <tableColumn id="4" name="full H"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица224" displayName="Таблица224" ref="A37:D51" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A37:D51"/>
   <tableColumns count="4">
     <tableColumn id="1" name="feature name"/>
     <tableColumn id="2" name="normal H"/>
@@ -480,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,224 +730,656 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>